<commit_message>
Commit 5 updating SEO
</commit_message>
<xml_diff>
--- a/documents/audit/audit SEO la panthere.xlsx
+++ b/documents/audit/audit SEO la panthere.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="66">
   <si>
     <t>Catégorie</t>
   </si>
@@ -84,15 +84,6 @@
     <t>definiton des width et des heights des images dans le code</t>
   </si>
   <si>
-    <t>visibilité des polices de caractère à l'affichage de la page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utilisez &lt;link rel="preload" as="font"&gt; pour appeler font </t>
-  </si>
-  <si>
-    <t>lenteur d'affichage des fonts</t>
-  </si>
-  <si>
     <t>4 liens vides(réseaux sociaux)</t>
   </si>
   <si>
@@ -123,9 +114,6 @@
     <t>convertion et réintégration des images au format  Webp ou AVIF</t>
   </si>
   <si>
-    <t>charger font sur fichier html</t>
-  </si>
-  <si>
     <t>réglage du contraste du texte aux normes en changeant la couleur de font</t>
   </si>
   <si>
@@ -138,21 +126,6 @@
     <t>https://www.codeur.com/tuto/html/attribut-a-href/</t>
   </si>
   <si>
-    <t>nombre de requete et taille transfert trop élevé</t>
-  </si>
-  <si>
-    <t>  budgets liés à la quantité et à la taille des ressources de pages trop important</t>
-  </si>
-  <si>
-    <t>ajoutez un fichier budget.json</t>
-  </si>
-  <si>
-    <t>  diminuer budgets liés à la quantité et à la taille des ressources de pages trop important</t>
-  </si>
-  <si>
-    <t>https://web.dev/use-lighthouse-for-performance-budgets/?utm_source=lighthouse&amp;utm_medium=lr</t>
-  </si>
-  <si>
     <t>redirection des href vers liens sociaux(noter du texte)</t>
   </si>
   <si>
@@ -171,34 +144,85 @@
     <t>textes à changer  en rapport avec l'image concernée</t>
   </si>
   <si>
-    <t>liens redondants</t>
-  </si>
-  <si>
-    <t>regrouper l'ensemble des liens</t>
-  </si>
-  <si>
-    <t>changer la redirection de chaque lien</t>
-  </si>
-  <si>
     <t>contrôle des polices de caractère pour être en conformité avec WCAG 2.0</t>
   </si>
   <si>
-    <t>7  liens se répètent des redirections similiraires</t>
-  </si>
-  <si>
     <t>https://web.dev/optimize-cls/?utm_source=lighthouse&amp;utm_medium=lr#images-without-dimensions</t>
   </si>
   <si>
-    <t>https://webaim.org/standards/wcag/checklist#sc2.4.4</t>
-  </si>
-  <si>
-    <t>https://web.dev/font-display/?utm_source=lighthouse&amp;utm_medium=lr</t>
-  </si>
-  <si>
     <t>https://a11y-guidelines.orange.com/fr/articles/couleur-et-taille-du-texte/</t>
   </si>
   <si>
     <t>https://webaim.org/standards/wcag/checklist#sc1.1.1</t>
+  </si>
+  <si>
+    <t>changement mots clés</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ajout balise meta robots </t>
+  </si>
+  <si>
+    <t>ajout balise meta canonical</t>
+  </si>
+  <si>
+    <t>keywords répétitifs et non optimisés à l'activité du site</t>
+  </si>
+  <si>
+    <t>choix de nouveaux keywords adaptés à l'activité deu site</t>
+  </si>
+  <si>
+    <t>remplacement de tous les keywords</t>
+  </si>
+  <si>
+    <t>https://smartkeyword.io/seo-technique-seo-balise-meta-robots/</t>
+  </si>
+  <si>
+    <t>absence de balise</t>
+  </si>
+  <si>
+    <t>absence de title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ajout balise </t>
+  </si>
+  <si>
+    <t>&lt;meta name="robots" content="index,follow"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;meta name="canonical"&gt;</t>
+  </si>
+  <si>
+    <t>https://developers.google.com/search/docs/advanced/crawling/consolidate-duplicate-urls?hl=fr</t>
+  </si>
+  <si>
+    <t>remplacement intitulés barre nav header sur  les 2 pages html</t>
+  </si>
+  <si>
+    <t>Transformation page 2 en contact sur pages html</t>
+  </si>
+  <si>
+    <t>problème  nommage  barre nav pour index et page2 html</t>
+  </si>
+  <si>
+    <t>page 2 inscrit sur les pages html alors que cela doit mener à la page "contact"</t>
+  </si>
+  <si>
+    <t>nommer le nom de la page web</t>
+  </si>
+  <si>
+    <t>titre donné: "la panthère agence, webdesign lyon"</t>
+  </si>
+  <si>
+    <t>absence de titre sur  balise title</t>
+  </si>
+  <si>
+    <t>https://www.semjuice.com/definition/balise-meta-keywords#:~:text=La%20balise%20meta%20Keywords%20est,obsol%C3%A8te%2C%20sans%20aucun%20int%C3%A9r%C3%AAt%20SEO.</t>
+  </si>
+  <si>
+    <t>https://fr.wix.com/blog/amp/2017/10/18/seo-comment-etre-bien-reference-sur-google-grace-a-vos-titres?utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=12441275269^119996084522&amp;experiment_id=^^501532539586^^_DSA&amp;gclid=CjwKCAjw3qGYBhBSEiwAcnTRLp8Ac-sUWsooEkU_0cOG0a9g6qA6buWAkAnR8RROpLsnNm5C_mLG_BoCCtEQAvD_BwE</t>
+  </si>
+  <si>
+    <t>https://www.mayboutik.com/connaitre-liens-internes-seo/</t>
   </si>
 </sst>
 </file>
@@ -243,17 +267,17 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF191919"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u/>
       <sz val="12"/>
       <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -326,9 +350,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -338,14 +359,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -358,6 +373,13 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -572,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -630,208 +652,246 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="50.1" customHeight="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="50.1" customHeight="1">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" s="13" customFormat="1" ht="50.1" customHeight="1">
+      <c r="A4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C4" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D4" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>36</v>
+      <c r="E4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="50.1" customHeight="1">
-      <c r="A4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="50.1" customHeight="1">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:26" s="13" customFormat="1" ht="50.1" customHeight="1">
+      <c r="A5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="12" t="s">
         <v>31</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="50.1" customHeight="1">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="9" t="s">
+      <c r="B6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" s="13" customFormat="1" ht="50.1" customHeight="1">
+      <c r="A7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" s="10" t="s">
+      <c r="F7" s="12" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="50.1" customHeight="1">
-      <c r="A7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="50.1" customHeight="1">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="81" customHeight="1">
+      <c r="A9" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="50.1" customHeight="1">
-      <c r="A9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>32</v>
-      </c>
       <c r="F9" s="8" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="50.1" customHeight="1">
-      <c r="A10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>51</v>
+      <c r="A10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>53</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="50.1" customHeight="1">
-      <c r="A11" s="6" t="s">
-        <v>12</v>
+      <c r="A11" s="9" t="s">
+        <v>6</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>47</v>
+        <v>52</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>54</v>
       </c>
       <c r="F11" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="132" customHeight="1">
+      <c r="A12" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="50.1" customHeight="1">
+      <c r="A13" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>57</v>
       </c>
+      <c r="F13" s="8" t="s">
+        <v>65</v>
+      </c>
     </row>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1"/>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1"/>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="14" spans="1:26" ht="30" customHeight="1"/>
     <row r="15" spans="1:26" ht="15.75" customHeight="1"/>
     <row r="16" spans="1:26" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
@@ -1816,23 +1876,22 @@
     <row r="996" ht="15.75" customHeight="1"/>
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
-    <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
     <hyperlink ref="F5" r:id="rId2"/>
     <hyperlink ref="F3" r:id="rId3"/>
-    <hyperlink ref="F6" r:id="rId4"/>
-    <hyperlink ref="F7" r:id="rId5" location="images-without-dimensions"/>
-    <hyperlink ref="F8" r:id="rId6" location="sc2.4.4"/>
-    <hyperlink ref="F9" r:id="rId7"/>
+    <hyperlink ref="F6" r:id="rId4" location="images-without-dimensions"/>
+    <hyperlink ref="F7" r:id="rId5"/>
+    <hyperlink ref="F8" r:id="rId6" location="sc1.1.1"/>
+    <hyperlink ref="F4" r:id="rId7"/>
     <hyperlink ref="F10" r:id="rId8"/>
-    <hyperlink ref="F11" r:id="rId9" location="sc1.1.1"/>
-    <hyperlink ref="F4" r:id="rId10"/>
+    <hyperlink ref="F11" r:id="rId9"/>
+    <hyperlink ref="F9" r:id="rId10" location=":~:text=La%20balise%20meta%20Keywords%20est,obsol%C3%A8te%2C%20sans%20aucun%20int%C3%A9r%C3%AAt%20SEO."/>
+    <hyperlink ref="F12"/>
+    <hyperlink ref="F13" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId11"/>
+  <pageSetup orientation="landscape" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
COMMIT 7 update all recommandations
</commit_message>
<xml_diff>
--- a/documents/audit/audit SEO la panthere.xlsx
+++ b/documents/audit/audit SEO la panthere.xlsx
@@ -280,7 +280,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -296,6 +296,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -338,7 +344,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -350,16 +356,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -374,11 +371,23 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -596,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -651,243 +660,243 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="50.1" customHeight="1">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:26" s="13" customFormat="1" ht="50.1" customHeight="1">
+      <c r="A2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="50.1" customHeight="1">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:26" s="13" customFormat="1" ht="50.1" customHeight="1">
+      <c r="A3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:26" s="13" customFormat="1" ht="50.1" customHeight="1">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="9" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:26" s="13" customFormat="1" ht="50.1" customHeight="1">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="50.1" customHeight="1">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:26" s="13" customFormat="1" ht="50.1" customHeight="1">
+      <c r="A6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="9" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:26" s="13" customFormat="1" ht="50.1" customHeight="1">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="50.1" customHeight="1">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:26" s="13" customFormat="1" ht="50.1" customHeight="1">
+      <c r="A8" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="81" customHeight="1">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:26" s="13" customFormat="1" ht="81" customHeight="1">
+      <c r="A9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="14" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="50.1" customHeight="1">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="14" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="50.1" customHeight="1">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="14" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="132" customHeight="1">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="14" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="50.1" customHeight="1">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="14" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>

<commit_message>
COMMIT UPDATE IMG TEXTE LINK HEADER FOOTER
</commit_message>
<xml_diff>
--- a/documents/audit/audit SEO la panthere.xlsx
+++ b/documents/audit/audit SEO la panthere.xlsx
@@ -72,9 +72,6 @@
     <t>poids trop lourd</t>
   </si>
   <si>
-    <t>convertir images en format nouvelle génération Webp ou AVIF</t>
-  </si>
-  <si>
     <t>widht et height non explicites sur les images</t>
   </si>
   <si>
@@ -102,18 +99,6 @@
     <t>modification du contraste pour le texte par rapport au background et aux normes WACG 2.0  (4,5:1)</t>
   </si>
   <si>
-    <t>taille de texte trop petite dans header</t>
-  </si>
-  <si>
-    <t>police de caractère trop basse</t>
-  </si>
-  <si>
-    <t>augmentation de la police de caractère</t>
-  </si>
-  <si>
-    <t>convertion et réintégration des images au format  Webp ou AVIF</t>
-  </si>
-  <si>
     <t>réglage du contraste du texte aux normes en changeant la couleur de font</t>
   </si>
   <si>
@@ -132,30 +117,9 @@
     <t>donner des width et height explicites aux images</t>
   </si>
   <si>
-    <t>texte identique pour 2 images à proximité</t>
-  </si>
-  <si>
-    <t>même légende sur 2 pages identiques</t>
-  </si>
-  <si>
-    <t>changer de manière significaitve les légendes des 2 images</t>
-  </si>
-  <si>
-    <t>textes à changer  en rapport avec l'image concernée</t>
-  </si>
-  <si>
-    <t>contrôle des polices de caractère pour être en conformité avec WCAG 2.0</t>
-  </si>
-  <si>
     <t>https://web.dev/optimize-cls/?utm_source=lighthouse&amp;utm_medium=lr#images-without-dimensions</t>
   </si>
   <si>
-    <t>https://a11y-guidelines.orange.com/fr/articles/couleur-et-taille-du-texte/</t>
-  </si>
-  <si>
-    <t>https://webaim.org/standards/wcag/checklist#sc1.1.1</t>
-  </si>
-  <si>
     <t>changement mots clés</t>
   </si>
   <si>
@@ -226,6 +190,42 @@
   </si>
   <si>
     <t>absence de balise &lt;meta name="canonical"&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">convertir images en format nouvelle génération en Webp </t>
+  </si>
+  <si>
+    <t xml:space="preserve">convertion et réintégration des images au format  en Webp </t>
+  </si>
+  <si>
+    <t>2 paragraphe sous forme d'image page accueil</t>
+  </si>
+  <si>
+    <t>Modification de 2 images à noter sous format texte</t>
+  </si>
+  <si>
+    <t>transformation des 2 images title et citation en texte</t>
+  </si>
+  <si>
+    <t>création de balise p pour changement des 2 images title et citation en format texte</t>
+  </si>
+  <si>
+    <t>dans header et footer balise keywords mots inadaptés et liens inutiles dans footer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> header et footer balise keywords et liens inutiles </t>
+  </si>
+  <si>
+    <t>suppression dans header et footer balise keywords  des mots inadaptés  et liens inutiles dans footer</t>
+  </si>
+  <si>
+    <t>changement dans header et footer balise keywords  des mots clés adaptés à l'activité pour référencement  et  suppressions des liens inutiles dans footer pour rapidité d'affichage</t>
+  </si>
+  <si>
+    <t>https://www.mygreatlearning.com/blog/the-access-modifiers-in-java/</t>
+  </si>
+  <si>
+    <t>https://www.blogdumoderateur.com/google-referencement-images-seo-conseils/</t>
   </si>
 </sst>
 </file>
@@ -347,7 +347,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -357,9 +357,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -372,15 +369,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -606,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="C8" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -663,247 +651,247 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" s="13" customFormat="1" ht="50.1" customHeight="1">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:26" s="9" customFormat="1" ht="50.1" customHeight="1">
+      <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="13" customFormat="1" ht="50.1" customHeight="1">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:26" s="9" customFormat="1" ht="50.1" customHeight="1">
+      <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" s="9" customFormat="1" ht="50.1" customHeight="1">
+      <c r="A4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="C4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" s="9" customFormat="1" ht="50.1" customHeight="1">
+      <c r="A5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" s="9" customFormat="1" ht="50.1" customHeight="1">
+      <c r="A6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" s="9" customFormat="1" ht="81" customHeight="1">
+      <c r="A7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="50.1" customHeight="1">
+      <c r="A8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="50.1" customHeight="1">
+      <c r="A9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>32</v>
+      <c r="C9" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:26" s="13" customFormat="1" ht="50.1" customHeight="1">
-      <c r="A4" s="10" t="s">
+    <row r="10" spans="1:26" ht="132" customHeight="1">
+      <c r="A10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>30</v>
+      <c r="B10" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:26" s="13" customFormat="1" ht="50.1" customHeight="1">
-      <c r="A5" s="11" t="s">
+    <row r="11" spans="1:26" ht="49.5" customHeight="1">
+      <c r="A11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="50.1" customHeight="1">
+      <c r="A12" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" s="13" customFormat="1" ht="50.1" customHeight="1">
-      <c r="A6" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" s="13" customFormat="1" ht="50.1" customHeight="1">
-      <c r="A7" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" s="13" customFormat="1" ht="50.1" customHeight="1">
-      <c r="A8" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" s="13" customFormat="1" ht="81" customHeight="1">
-      <c r="A9" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="14" t="s">
+      <c r="B12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="10" spans="1:26" ht="50.1" customHeight="1">
-      <c r="A10" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="50.1" customHeight="1">
-      <c r="A11" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="8" t="s">
+      <c r="F12" s="10" t="s">
         <v>66</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="132" customHeight="1">
-      <c r="A12" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="50.1" customHeight="1">
-      <c r="A13" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F13" s="14" t="s">
+      <c r="A13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>62</v>
       </c>
+      <c r="C13" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>65</v>
+      </c>
     </row>
-    <row r="14" spans="1:26" ht="30" customHeight="1"/>
+    <row r="14" spans="1:26" ht="15.75" customHeight="1"/>
     <row r="15" spans="1:26" ht="15.75" customHeight="1"/>
     <row r="16" spans="1:26" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
@@ -1886,22 +1874,20 @@
     <row r="994" ht="15.75" customHeight="1"/>
     <row r="995" ht="15.75" customHeight="1"/>
     <row r="996" ht="15.75" customHeight="1"/>
-    <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
     <hyperlink ref="F5" r:id="rId2"/>
     <hyperlink ref="F3" r:id="rId3"/>
     <hyperlink ref="F6" r:id="rId4" location="images-without-dimensions"/>
-    <hyperlink ref="F7" r:id="rId5"/>
-    <hyperlink ref="F8" r:id="rId6" location="sc1.1.1"/>
-    <hyperlink ref="F4" r:id="rId7"/>
-    <hyperlink ref="F10" r:id="rId8"/>
+    <hyperlink ref="F4" r:id="rId5"/>
+    <hyperlink ref="F8" r:id="rId6"/>
+    <hyperlink ref="F9" r:id="rId7"/>
+    <hyperlink ref="F7" r:id="rId8" location=":~:text=La%20balise%20meta%20Keywords%20est,obsol%C3%A8te%2C%20sans%20aucun%20int%C3%A9r%C3%AAt%20SEO."/>
+    <hyperlink ref="F10" display="https://fr.wix.com/blog/amp/2017/10/18/seo-comment-etre-bien-reference-sur-google-grace-a-vos-titres?utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=12441275269^119996084522&amp;experiment_id=^^501532539586^^_DSA&amp;gclid=CjwKCAjw3qGYBhBSEiwAcnTRLp8Ac-sUWsooEkU_0c"/>
     <hyperlink ref="F11" r:id="rId9"/>
-    <hyperlink ref="F9" r:id="rId10" location=":~:text=La%20balise%20meta%20Keywords%20est,obsol%C3%A8te%2C%20sans%20aucun%20int%C3%A9r%C3%AAt%20SEO."/>
-    <hyperlink ref="F12" display="https://fr.wix.com/blog/amp/2017/10/18/seo-comment-etre-bien-reference-sur-google-grace-a-vos-titres?utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=12441275269^119996084522&amp;experiment_id=^^501532539586^^_DSA&amp;gclid=CjwKCAjw3qGYBhBSEiwAcnTRLp8Ac-sUWsooEkU_0c"/>
-    <hyperlink ref="F13" r:id="rId11"/>
+    <hyperlink ref="F13" r:id="rId10"/>
+    <hyperlink ref="F12" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId12"/>

</xml_diff>

<commit_message>
commit 13 link social updating
</commit_message>
<xml_diff>
--- a/documents/audit/audit SEO la panthere.xlsx
+++ b/documents/audit/audit SEO la panthere.xlsx
@@ -90,15 +90,9 @@
     <t>faire des href pour les liens concernés pour redirection</t>
   </si>
   <si>
-    <t xml:space="preserve">contrastre texte non conforme </t>
-  </si>
-  <si>
     <t>contraste invalide pour le texte par rapport au background</t>
   </si>
   <si>
-    <t>modification du contraste pour le texte par rapport au background et aux normes WACG 2.0  (4,5:1)</t>
-  </si>
-  <si>
     <t>réglage du contraste du texte aux normes en changeant la couleur de font</t>
   </si>
   <si>
@@ -226,6 +220,12 @@
   </si>
   <si>
     <t>https://www.blogdumoderateur.com/google-referencement-images-seo-conseils/</t>
+  </si>
+  <si>
+    <t>adapter le contraste pour le texte par rapport au background et aux normes WACG 2.0  (4,5:1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contraste texte non conforme </t>
   </si>
 </sst>
 </file>
@@ -596,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C8" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -685,10 +685,10 @@
         <v>20</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:26" s="9" customFormat="1" ht="50.1" customHeight="1">
@@ -696,19 +696,19 @@
         <v>6</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="D4" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="F4" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:26" s="9" customFormat="1" ht="50.1" customHeight="1">
@@ -722,13 +722,13 @@
         <v>14</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:26" s="9" customFormat="1" ht="50.1" customHeight="1">
@@ -745,10 +745,10 @@
         <v>17</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:26" s="9" customFormat="1" ht="81" customHeight="1">
@@ -756,19 +756,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>36</v>
-      </c>
       <c r="F7" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="50.1" customHeight="1">
@@ -776,19 +776,19 @@
         <v>6</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="50.1" customHeight="1">
@@ -796,19 +796,19 @@
         <v>6</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="132" customHeight="1">
@@ -816,19 +816,19 @@
         <v>6</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="10" t="s">
         <v>47</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="49.5" customHeight="1">
@@ -836,19 +836,19 @@
         <v>6</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="50.1" customHeight="1">
@@ -856,19 +856,19 @@
         <v>12</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="E12" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>60</v>
-      </c>
       <c r="F12" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="50.1" customHeight="1">
@@ -876,19 +876,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="7" t="s">
+      <c r="F13" s="10" t="s">
         <v>63</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1"/>

</xml_diff>